<commit_message>
Started the write up
</commit_message>
<xml_diff>
--- a/Polorization Data.xlsx
+++ b/Polorization Data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tymarking/Documents/Polarization_Lab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mass Storage\School Work (Current Year)\11th Grade\Physics C Mechanics\Polarization_Lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6339941F-F671-1F43-B6D9-715ABBC38534}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FCBE40-8B7C-41B0-9CC6-6BB29E03ABE8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{E84BFA19-DF2A-4658-93B1-E1C0ADF996B3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{E84BFA19-DF2A-4658-93B1-E1C0ADF996B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t>Manipulated Variable</t>
   </si>
@@ -281,7 +282,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -4561,19 +4592,42 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8161D8B5-C0FA-2843-A9B1-2A848F333F46}" name="Table1" displayName="Table1" ref="C6:L45" totalsRowShown="0">
   <autoFilter ref="C6:L45" xr:uid="{E58AE203-B932-0B4D-84AA-EC78488D6452}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{7A4644D8-4EB5-C148-A144-13E6143BA73C}" name="Difference in filter orientation" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{1FE0CCF9-3C36-E345-AB20-6C538FA866AF}" name="Trial 1" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{7A4644D8-4EB5-C148-A144-13E6143BA73C}" name="Difference in filter orientation" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{1FE0CCF9-3C36-E345-AB20-6C538FA866AF}" name="Trial 1" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{10833C12-C981-EA4C-8118-E8C5E9C8CACD}" name="Trial 2"/>
     <tableColumn id="4" xr3:uid="{D3E7A334-D93E-1841-9997-35E2EAA1B253}" name="Trial 3"/>
     <tableColumn id="5" xr3:uid="{E84B53B0-CAAD-F540-865F-75C979B55C40}" name="Trial 4"/>
     <tableColumn id="6" xr3:uid="{143B88BD-7575-3546-86BE-0D27B8B2951F}" name="Trial 5"/>
     <tableColumn id="7" xr3:uid="{B708DF02-AA00-3A46-974E-DAF1BB525295}" name="Trial 6"/>
-    <tableColumn id="8" xr3:uid="{EC2D9506-430D-6143-AE51-FF6F103B06E3}" name="Trial 7" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{B12CB6DD-9531-0E45-893D-86B94EDC8415}" name="Average" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{EC2D9506-430D-6143-AE51-FF6F103B06E3}" name="Trial 7" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{B12CB6DD-9531-0E45-893D-86B94EDC8415}" name="Average" dataDxfId="4">
       <calculatedColumnFormula>AVERAGE(D7:J7)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{2600DC50-C1A5-2045-9565-2C68D6695A2D}" name="Deviation">
       <calculatedColumnFormula array="1">MAX(ABS(D7:J7-(ROUND(K7,0))))</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{76D54006-72EF-4A30-A21E-067EBE83A002}" name="Table14" displayName="Table14" ref="A1:J40" totalsRowShown="0">
+  <autoFilter ref="A1:J40" xr:uid="{3DE8E5C6-1C90-43D6-A51C-93D8183ADEB8}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{E51D4EAB-E5B8-45E1-AD42-DCAA8A5C36A5}" name="Difference in filter orientation" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{64FD89F2-2282-4B4A-99EF-BC54D75FC0F0}" name="Trial 1" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{09CCB193-28DE-4CB8-AB01-6367CD5D959D}" name="Trial 2"/>
+    <tableColumn id="4" xr3:uid="{F23D3549-3204-4097-937A-7D55233D29FF}" name="Trial 3"/>
+    <tableColumn id="5" xr3:uid="{086DE93D-C3E3-4739-BE4E-C9D1A290D2BF}" name="Trial 4"/>
+    <tableColumn id="6" xr3:uid="{A5F0C18B-3671-4953-B555-8087790EE799}" name="Trial 5"/>
+    <tableColumn id="7" xr3:uid="{1E73E82D-D824-4B15-AF13-A6676E5AF12E}" name="Trial 6"/>
+    <tableColumn id="8" xr3:uid="{C8289541-29B9-42D0-8C2B-94D44593ED8B}" name="Trial 7" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{CF3F48F2-ED75-4AE3-95BD-E9AA84CDBA1A}" name="Average" dataDxfId="0">
+      <calculatedColumnFormula>AVERAGE(B2:H2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{B5A8752D-9DDD-46C7-8ED4-03AF05A99333}" name="Deviation">
+      <calculatedColumnFormula array="1">MAX(ABS(B2:H2-(ROUND(I2,0))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4879,27 +4933,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03D581FF-A40B-4BD6-A21F-95CC15305563}">
   <dimension ref="C5:X139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:L45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
     <col min="8" max="10" width="10" customWidth="1"/>
-    <col min="11" max="11" width="10.5" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" customWidth="1"/>
-    <col min="16" max="16" width="8.83203125" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:24" x14ac:dyDescent="0.25">
       <c r="G5" s="19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>14</v>
       </c>
@@ -4943,7 +4997,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>1</v>
       </c>
@@ -4963,7 +5017,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="3:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
@@ -4991,7 +5045,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <v>0</v>
       </c>
@@ -5055,7 +5109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <v>10</v>
       </c>
@@ -5119,7 +5173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <v>20</v>
       </c>
@@ -5183,7 +5237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <v>30</v>
       </c>
@@ -5247,7 +5301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <v>40</v>
       </c>
@@ -5311,7 +5365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <v>50</v>
       </c>
@@ -5375,7 +5429,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <v>60</v>
       </c>
@@ -5439,7 +5493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <v>70</v>
       </c>
@@ -5503,7 +5557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <v>80</v>
       </c>
@@ -5567,7 +5621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <v>90</v>
       </c>
@@ -5631,7 +5685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <v>100</v>
       </c>
@@ -5695,7 +5749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <v>110</v>
       </c>
@@ -5759,7 +5813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <v>120</v>
       </c>
@@ -5823,7 +5877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <v>130</v>
       </c>
@@ -5887,7 +5941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <v>140</v>
       </c>
@@ -5951,7 +6005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <v>150</v>
       </c>
@@ -6015,7 +6069,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <v>160</v>
       </c>
@@ -6079,7 +6133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <v>170</v>
       </c>
@@ -6143,7 +6197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <v>180</v>
       </c>
@@ -6207,7 +6261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <v>190</v>
       </c>
@@ -6271,7 +6325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <v>200</v>
       </c>
@@ -6335,7 +6389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <v>210</v>
       </c>
@@ -6399,7 +6453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <v>220</v>
       </c>
@@ -6463,7 +6517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <v>230</v>
       </c>
@@ -6527,7 +6581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <v>240</v>
       </c>
@@ -6591,7 +6645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
         <v>250</v>
       </c>
@@ -6655,7 +6709,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
         <v>260</v>
       </c>
@@ -6719,7 +6773,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <v>270</v>
       </c>
@@ -6783,7 +6837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <v>280</v>
       </c>
@@ -6847,7 +6901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <v>290</v>
       </c>
@@ -6911,7 +6965,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
         <v>300</v>
       </c>
@@ -6975,7 +7029,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
         <v>310</v>
       </c>
@@ -7039,7 +7093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
         <v>320</v>
       </c>
@@ -7103,7 +7157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
         <v>330</v>
       </c>
@@ -7167,7 +7221,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
         <v>340</v>
       </c>
@@ -7231,7 +7285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
         <v>350</v>
       </c>
@@ -7295,7 +7349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="3:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C45" s="2">
         <v>360</v>
       </c>
@@ -7359,12 +7413,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:24" x14ac:dyDescent="0.25">
       <c r="E48">
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>20</v>
       </c>
@@ -7375,7 +7429,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C50" s="15">
         <v>0</v>
       </c>
@@ -7388,7 +7442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C51" s="16">
         <v>10</v>
       </c>
@@ -7401,7 +7455,7 @@
         <v>5.7291914453192163</v>
       </c>
     </row>
-    <row r="52" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C52" s="15">
         <v>20</v>
       </c>
@@ -7420,7 +7474,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="53" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C53" s="16">
         <v>30</v>
       </c>
@@ -7439,7 +7493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C54" s="15">
         <v>40</v>
       </c>
@@ -7458,7 +7512,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C55" s="16">
         <v>50</v>
       </c>
@@ -7477,7 +7531,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C56" s="15">
         <v>60</v>
       </c>
@@ -7496,7 +7550,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C57" s="16">
         <v>70</v>
       </c>
@@ -7515,7 +7569,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C58" s="15">
         <v>80</v>
       </c>
@@ -7534,7 +7588,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C59" s="16">
         <v>90</v>
       </c>
@@ -7553,7 +7607,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="60" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C60" s="15">
         <v>100</v>
       </c>
@@ -7572,7 +7626,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="61" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C61" s="16">
         <v>110</v>
       </c>
@@ -7591,7 +7645,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="62" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C62" s="15">
         <v>120</v>
       </c>
@@ -7610,7 +7664,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="63" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C63" s="16">
         <v>130</v>
       </c>
@@ -7629,7 +7683,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="64" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C64" s="15">
         <v>140</v>
       </c>
@@ -7648,7 +7702,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="65" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C65" s="16">
         <v>150</v>
       </c>
@@ -7667,7 +7721,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="66" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C66" s="15">
         <v>160</v>
       </c>
@@ -7686,7 +7740,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C67" s="16">
         <v>170</v>
       </c>
@@ -7705,7 +7759,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C68" s="15">
         <v>180</v>
       </c>
@@ -7724,7 +7778,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C69" s="16">
         <v>190</v>
       </c>
@@ -7743,7 +7797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C70" s="15">
         <v>200</v>
       </c>
@@ -7762,7 +7816,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="71" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C71" s="16">
         <v>210</v>
       </c>
@@ -7781,7 +7835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C72" s="15">
         <v>220</v>
       </c>
@@ -7800,7 +7854,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C73" s="16">
         <v>230</v>
       </c>
@@ -7819,7 +7873,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="74" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C74" s="15">
         <v>240</v>
       </c>
@@ -7838,7 +7892,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C75" s="16">
         <v>250</v>
       </c>
@@ -7857,7 +7911,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="76" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C76" s="15">
         <v>260</v>
       </c>
@@ -7876,7 +7930,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="77" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C77" s="16">
         <v>270</v>
       </c>
@@ -7895,7 +7949,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="78" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C78" s="15">
         <v>280</v>
       </c>
@@ -7914,7 +7968,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="79" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C79" s="16">
         <v>290</v>
       </c>
@@ -7933,7 +7987,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="80" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C80" s="15">
         <v>300</v>
       </c>
@@ -7952,7 +8006,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="81" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C81" s="16">
         <v>310</v>
       </c>
@@ -7971,7 +8025,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="82" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C82" s="15">
         <v>320</v>
       </c>
@@ -7990,7 +8044,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="83" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C83" s="16">
         <v>330</v>
       </c>
@@ -8009,7 +8063,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="84" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C84" s="15">
         <v>340</v>
       </c>
@@ -8028,7 +8082,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="85" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C85" s="16">
         <v>350</v>
       </c>
@@ -8047,7 +8101,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="86" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C86" s="15">
         <v>360</v>
       </c>
@@ -8066,7 +8120,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="3:10" x14ac:dyDescent="0.25">
       <c r="I87">
         <v>7</v>
       </c>
@@ -8074,7 +8128,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="3:10" x14ac:dyDescent="0.25">
       <c r="I88">
         <v>-1</v>
       </c>
@@ -8082,7 +8136,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="103" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D103" s="15">
         <v>0</v>
       </c>
@@ -8090,7 +8144,7 @@
         <v>-0.8571428571428571</v>
       </c>
     </row>
-    <row r="104" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D104" s="16">
         <v>10</v>
       </c>
@@ -8098,7 +8152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D105" s="15">
         <v>20</v>
       </c>
@@ -8106,7 +8160,7 @@
         <v>16.714285714285715</v>
       </c>
     </row>
-    <row r="106" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D106" s="16">
         <v>30</v>
       </c>
@@ -8114,7 +8168,7 @@
         <v>39.571428571428569</v>
       </c>
     </row>
-    <row r="107" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D107" s="15">
         <v>40</v>
       </c>
@@ -8122,7 +8176,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="108" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D108" s="16">
         <v>50</v>
       </c>
@@ -8130,7 +8184,7 @@
         <v>103.71428571428571</v>
       </c>
     </row>
-    <row r="109" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D109" s="15">
         <v>60</v>
       </c>
@@ -8138,7 +8192,7 @@
         <v>135.71428571428572</v>
       </c>
     </row>
-    <row r="110" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D110" s="16">
         <v>70</v>
       </c>
@@ -8146,7 +8200,7 @@
         <v>160.42857142857142</v>
       </c>
     </row>
-    <row r="111" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D111" s="15">
         <v>80</v>
       </c>
@@ -8154,7 +8208,7 @@
         <v>178.14285714285714</v>
       </c>
     </row>
-    <row r="112" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D112" s="16">
         <v>90</v>
       </c>
@@ -8162,7 +8216,7 @@
         <v>186.14285714285714</v>
       </c>
     </row>
-    <row r="113" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D113" s="15">
         <v>100</v>
       </c>
@@ -8170,7 +8224,7 @@
         <v>182.71428571428572</v>
       </c>
     </row>
-    <row r="114" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D114" s="16">
         <v>110</v>
       </c>
@@ -8178,7 +8232,7 @@
         <v>169.28571428571428</v>
       </c>
     </row>
-    <row r="115" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D115" s="15">
         <v>120</v>
       </c>
@@ -8186,7 +8240,7 @@
         <v>146.14285714285714</v>
       </c>
     </row>
-    <row r="116" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D116" s="16">
         <v>130</v>
       </c>
@@ -8194,7 +8248,7 @@
         <v>115.42857142857143</v>
       </c>
     </row>
-    <row r="117" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D117" s="15">
         <v>140</v>
       </c>
@@ -8202,7 +8256,7 @@
         <v>84.571428571428569</v>
       </c>
     </row>
-    <row r="118" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D118" s="16">
         <v>150</v>
       </c>
@@ -8210,7 +8264,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="119" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D119" s="15">
         <v>160</v>
       </c>
@@ -8218,7 +8272,7 @@
         <v>25.285714285714285</v>
       </c>
     </row>
-    <row r="120" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D120" s="16">
         <v>170</v>
       </c>
@@ -8226,7 +8280,7 @@
         <v>7.1428571428571432</v>
       </c>
     </row>
-    <row r="121" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D121" s="15">
         <v>180</v>
       </c>
@@ -8234,7 +8288,7 @@
         <v>-0.8571428571428571</v>
       </c>
     </row>
-    <row r="122" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D122" s="16">
         <v>190</v>
       </c>
@@ -8242,7 +8296,7 @@
         <v>1.4285714285714286</v>
       </c>
     </row>
-    <row r="123" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D123" s="15">
         <v>200</v>
       </c>
@@ -8250,7 +8304,7 @@
         <v>15.142857142857142</v>
       </c>
     </row>
-    <row r="124" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D124" s="16">
         <v>210</v>
       </c>
@@ -8258,7 +8312,7 @@
         <v>39.285714285714285</v>
       </c>
     </row>
-    <row r="125" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D125" s="15">
         <v>220</v>
       </c>
@@ -8266,7 +8320,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="126" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D126" s="16">
         <v>230</v>
       </c>
@@ -8274,7 +8328,7 @@
         <v>102.42857142857143</v>
       </c>
     </row>
-    <row r="127" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D127" s="15">
         <v>240</v>
       </c>
@@ -8282,7 +8336,7 @@
         <v>137.71428571428572</v>
       </c>
     </row>
-    <row r="128" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D128" s="16">
         <v>250</v>
       </c>
@@ -8290,7 +8344,7 @@
         <v>165.42857142857142</v>
       </c>
     </row>
-    <row r="129" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D129" s="15">
         <v>260</v>
       </c>
@@ -8298,7 +8352,7 @@
         <v>189.28571428571428</v>
       </c>
     </row>
-    <row r="130" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D130" s="16">
         <v>270</v>
       </c>
@@ -8306,7 +8360,7 @@
         <v>202.57142857142858</v>
       </c>
     </row>
-    <row r="131" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D131" s="15">
         <v>280</v>
       </c>
@@ -8314,7 +8368,7 @@
         <v>200.57142857142858</v>
       </c>
     </row>
-    <row r="132" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D132" s="16">
         <v>290</v>
       </c>
@@ -8322,7 +8376,7 @@
         <v>186.14285714285714</v>
       </c>
     </row>
-    <row r="133" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D133" s="15">
         <v>300</v>
       </c>
@@ -8330,7 +8384,7 @@
         <v>160.42857142857142</v>
       </c>
     </row>
-    <row r="134" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D134" s="16">
         <v>310</v>
       </c>
@@ -8338,7 +8392,7 @@
         <v>124.28571428571429</v>
       </c>
     </row>
-    <row r="135" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D135" s="15">
         <v>320</v>
       </c>
@@ -8346,7 +8400,7 @@
         <v>89.571428571428569</v>
       </c>
     </row>
-    <row r="136" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D136" s="16">
         <v>330</v>
       </c>
@@ -8354,7 +8408,7 @@
         <v>54.714285714285715</v>
       </c>
     </row>
-    <row r="137" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D137" s="15">
         <v>340</v>
       </c>
@@ -8362,7 +8416,7 @@
         <v>25.571428571428573</v>
       </c>
     </row>
-    <row r="138" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D138" s="16">
         <v>350</v>
       </c>
@@ -8370,7 +8424,7 @@
         <v>7.1428571428571432</v>
       </c>
     </row>
-    <row r="139" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D139" s="15">
         <v>360</v>
       </c>
@@ -8385,4 +8439,1336 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89373B48-D580-415D-8340-2D7F51AF4F0B}">
+  <dimension ref="A1:J40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="11"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>-1</v>
+      </c>
+      <c r="G4" s="7">
+        <v>-1</v>
+      </c>
+      <c r="H4" s="8">
+        <v>-1</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" ref="I4:I40" si="0">AVERAGE(B4:H4)</f>
+        <v>-0.8571428571428571</v>
+      </c>
+      <c r="J4">
+        <f t="array" ref="J4">MAX(ABS(B4:H4-(ROUND(I4,0))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>10</v>
+      </c>
+      <c r="B5" s="9">
+        <v>2</v>
+      </c>
+      <c r="C5" s="10">
+        <v>3</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10">
+        <v>2</v>
+      </c>
+      <c r="F5" s="10">
+        <v>2</v>
+      </c>
+      <c r="G5" s="10">
+        <v>2</v>
+      </c>
+      <c r="H5" s="11">
+        <v>2</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <f t="array" ref="J5">MAX(ABS(B5:H5-(ROUND(I5,0))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>20</v>
+      </c>
+      <c r="B6" s="9">
+        <v>16</v>
+      </c>
+      <c r="C6" s="10">
+        <v>17</v>
+      </c>
+      <c r="D6" s="10">
+        <v>17</v>
+      </c>
+      <c r="E6" s="10">
+        <v>16</v>
+      </c>
+      <c r="F6" s="10">
+        <v>17</v>
+      </c>
+      <c r="G6" s="10">
+        <v>16</v>
+      </c>
+      <c r="H6" s="11">
+        <v>18</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" si="0"/>
+        <v>16.714285714285715</v>
+      </c>
+      <c r="J6">
+        <f t="array" ref="J6">MAX(ABS(B6:H6-(ROUND(I6,0))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>30</v>
+      </c>
+      <c r="B7" s="9">
+        <v>39</v>
+      </c>
+      <c r="C7" s="10">
+        <v>41</v>
+      </c>
+      <c r="D7" s="10">
+        <v>37</v>
+      </c>
+      <c r="E7" s="10">
+        <v>41</v>
+      </c>
+      <c r="F7" s="10">
+        <v>39</v>
+      </c>
+      <c r="G7" s="10">
+        <v>38</v>
+      </c>
+      <c r="H7" s="11">
+        <v>42</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" si="0"/>
+        <v>39.571428571428569</v>
+      </c>
+      <c r="J7">
+        <f t="array" ref="J7">MAX(ABS(B7:H7-(ROUND(I7,0))))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>40</v>
+      </c>
+      <c r="B8" s="9">
+        <v>69</v>
+      </c>
+      <c r="C8" s="10">
+        <v>70</v>
+      </c>
+      <c r="D8" s="10">
+        <v>69</v>
+      </c>
+      <c r="E8" s="10">
+        <v>70</v>
+      </c>
+      <c r="F8" s="10">
+        <v>70</v>
+      </c>
+      <c r="G8" s="10">
+        <v>71</v>
+      </c>
+      <c r="H8" s="11">
+        <v>71</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="J8">
+        <f t="array" ref="J8">MAX(ABS(B8:H8-(ROUND(I8,0))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>50</v>
+      </c>
+      <c r="B9" s="9">
+        <v>103</v>
+      </c>
+      <c r="C9" s="10">
+        <v>104</v>
+      </c>
+      <c r="D9" s="10">
+        <v>102</v>
+      </c>
+      <c r="E9" s="10">
+        <v>100</v>
+      </c>
+      <c r="F9" s="10">
+        <v>103</v>
+      </c>
+      <c r="G9" s="10">
+        <v>106</v>
+      </c>
+      <c r="H9" s="11">
+        <v>108</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="0"/>
+        <v>103.71428571428571</v>
+      </c>
+      <c r="J9">
+        <f t="array" ref="J9">MAX(ABS(B9:H9-(ROUND(I9,0))))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>60</v>
+      </c>
+      <c r="B10" s="9">
+        <v>133</v>
+      </c>
+      <c r="C10" s="10">
+        <v>135</v>
+      </c>
+      <c r="D10" s="10">
+        <v>137</v>
+      </c>
+      <c r="E10" s="10">
+        <v>135</v>
+      </c>
+      <c r="F10" s="10">
+        <v>133</v>
+      </c>
+      <c r="G10" s="10">
+        <v>134</v>
+      </c>
+      <c r="H10" s="11">
+        <v>143</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" si="0"/>
+        <v>135.71428571428572</v>
+      </c>
+      <c r="J10">
+        <f t="array" ref="J10">MAX(ABS(B10:H10-(ROUND(I10,0))))</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>70</v>
+      </c>
+      <c r="B11" s="9">
+        <v>160</v>
+      </c>
+      <c r="C11" s="10">
+        <v>161</v>
+      </c>
+      <c r="D11" s="10">
+        <v>158</v>
+      </c>
+      <c r="E11" s="10">
+        <v>159</v>
+      </c>
+      <c r="F11" s="10">
+        <v>158</v>
+      </c>
+      <c r="G11" s="10">
+        <v>159</v>
+      </c>
+      <c r="H11" s="11">
+        <v>168</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" si="0"/>
+        <v>160.42857142857142</v>
+      </c>
+      <c r="J11">
+        <f t="array" ref="J11">MAX(ABS(B11:H11-(ROUND(I11,0))))</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>80</v>
+      </c>
+      <c r="B12" s="9">
+        <v>177</v>
+      </c>
+      <c r="C12" s="10">
+        <v>177</v>
+      </c>
+      <c r="D12" s="10">
+        <v>177</v>
+      </c>
+      <c r="E12" s="10">
+        <v>176</v>
+      </c>
+      <c r="F12" s="10">
+        <v>176</v>
+      </c>
+      <c r="G12" s="10">
+        <v>176</v>
+      </c>
+      <c r="H12" s="11">
+        <v>188</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" si="0"/>
+        <v>178.14285714285714</v>
+      </c>
+      <c r="J12">
+        <f t="array" ref="J12">MAX(ABS(B12:H12-(ROUND(I12,0))))</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>90</v>
+      </c>
+      <c r="B13" s="9">
+        <v>184</v>
+      </c>
+      <c r="C13" s="10">
+        <v>185</v>
+      </c>
+      <c r="D13" s="10">
+        <v>184</v>
+      </c>
+      <c r="E13" s="10">
+        <v>185</v>
+      </c>
+      <c r="F13" s="10">
+        <v>183</v>
+      </c>
+      <c r="G13" s="10">
+        <v>184</v>
+      </c>
+      <c r="H13" s="11">
+        <v>198</v>
+      </c>
+      <c r="I13" s="3">
+        <f t="shared" si="0"/>
+        <v>186.14285714285714</v>
+      </c>
+      <c r="J13">
+        <f t="array" ref="J13">MAX(ABS(B13:H13-(ROUND(I13,0))))</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>100</v>
+      </c>
+      <c r="B14" s="9">
+        <v>181</v>
+      </c>
+      <c r="C14" s="10">
+        <v>182</v>
+      </c>
+      <c r="D14" s="10">
+        <v>181</v>
+      </c>
+      <c r="E14" s="10">
+        <v>181</v>
+      </c>
+      <c r="F14" s="10">
+        <v>180</v>
+      </c>
+      <c r="G14" s="10">
+        <v>180</v>
+      </c>
+      <c r="H14" s="11">
+        <v>194</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" si="0"/>
+        <v>182.71428571428572</v>
+      </c>
+      <c r="J14">
+        <f t="array" ref="J14">MAX(ABS(B14:H14-(ROUND(I14,0))))</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>110</v>
+      </c>
+      <c r="B15" s="9">
+        <v>168</v>
+      </c>
+      <c r="C15" s="10">
+        <v>167</v>
+      </c>
+      <c r="D15" s="10">
+        <v>169</v>
+      </c>
+      <c r="E15" s="10">
+        <v>168</v>
+      </c>
+      <c r="F15" s="10">
+        <v>165</v>
+      </c>
+      <c r="G15" s="10">
+        <v>167</v>
+      </c>
+      <c r="H15" s="11">
+        <v>181</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" si="0"/>
+        <v>169.28571428571428</v>
+      </c>
+      <c r="J15">
+        <f t="array" ref="J15">MAX(ABS(B15:H15-(ROUND(I15,0))))</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>120</v>
+      </c>
+      <c r="B16" s="9">
+        <v>145</v>
+      </c>
+      <c r="C16" s="10">
+        <v>145</v>
+      </c>
+      <c r="D16" s="10">
+        <v>145</v>
+      </c>
+      <c r="E16" s="10">
+        <v>144</v>
+      </c>
+      <c r="F16" s="10">
+        <v>145</v>
+      </c>
+      <c r="G16" s="10">
+        <v>142</v>
+      </c>
+      <c r="H16" s="11">
+        <v>157</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="0"/>
+        <v>146.14285714285714</v>
+      </c>
+      <c r="J16">
+        <f t="array" ref="J16">MAX(ABS(B16:H16-(ROUND(I16,0))))</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>130</v>
+      </c>
+      <c r="B17" s="9">
+        <v>117</v>
+      </c>
+      <c r="C17" s="10">
+        <v>114</v>
+      </c>
+      <c r="D17" s="10">
+        <v>115</v>
+      </c>
+      <c r="E17" s="10">
+        <v>114</v>
+      </c>
+      <c r="F17" s="10">
+        <v>113</v>
+      </c>
+      <c r="G17" s="10">
+        <v>112</v>
+      </c>
+      <c r="H17" s="11">
+        <v>123</v>
+      </c>
+      <c r="I17" s="3">
+        <f t="shared" si="0"/>
+        <v>115.42857142857143</v>
+      </c>
+      <c r="J17">
+        <f t="array" ref="J17">MAX(ABS(B17:H17-(ROUND(I17,0))))</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>140</v>
+      </c>
+      <c r="B18" s="9">
+        <v>86</v>
+      </c>
+      <c r="C18" s="10">
+        <v>82</v>
+      </c>
+      <c r="D18" s="10">
+        <v>85</v>
+      </c>
+      <c r="E18" s="10">
+        <v>83</v>
+      </c>
+      <c r="F18" s="10">
+        <v>84</v>
+      </c>
+      <c r="G18" s="10">
+        <v>83</v>
+      </c>
+      <c r="H18" s="11">
+        <v>89</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" si="0"/>
+        <v>84.571428571428569</v>
+      </c>
+      <c r="J18">
+        <f t="array" ref="J18">MAX(ABS(B18:H18-(ROUND(I18,0))))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>150</v>
+      </c>
+      <c r="B19" s="9">
+        <v>55</v>
+      </c>
+      <c r="C19" s="10">
+        <v>52</v>
+      </c>
+      <c r="D19" s="10">
+        <v>53</v>
+      </c>
+      <c r="E19" s="10">
+        <v>54</v>
+      </c>
+      <c r="F19" s="10">
+        <v>52</v>
+      </c>
+      <c r="G19" s="10">
+        <v>52</v>
+      </c>
+      <c r="H19" s="11">
+        <v>53</v>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="J19">
+        <f t="array" ref="J19">MAX(ABS(B19:H19-(ROUND(I19,0))))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>160</v>
+      </c>
+      <c r="B20" s="9">
+        <v>25</v>
+      </c>
+      <c r="C20" s="10">
+        <v>24</v>
+      </c>
+      <c r="D20" s="10">
+        <v>26</v>
+      </c>
+      <c r="E20" s="10">
+        <v>25</v>
+      </c>
+      <c r="F20" s="10">
+        <v>24</v>
+      </c>
+      <c r="G20" s="10">
+        <v>27</v>
+      </c>
+      <c r="H20" s="11">
+        <v>26</v>
+      </c>
+      <c r="I20" s="3">
+        <f t="shared" si="0"/>
+        <v>25.285714285714285</v>
+      </c>
+      <c r="J20">
+        <f t="array" ref="J20">MAX(ABS(B20:H20-(ROUND(I20,0))))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>170</v>
+      </c>
+      <c r="B21" s="9">
+        <v>7</v>
+      </c>
+      <c r="C21" s="10">
+        <v>7</v>
+      </c>
+      <c r="D21" s="10">
+        <v>6</v>
+      </c>
+      <c r="E21" s="10">
+        <v>7</v>
+      </c>
+      <c r="F21" s="10">
+        <v>8</v>
+      </c>
+      <c r="G21" s="10">
+        <v>7</v>
+      </c>
+      <c r="H21" s="11">
+        <v>8</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" si="0"/>
+        <v>7.1428571428571432</v>
+      </c>
+      <c r="J21">
+        <f t="array" ref="J21">MAX(ABS(B21:H21-(ROUND(I21,0))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>180</v>
+      </c>
+      <c r="B22" s="9">
+        <v>-1</v>
+      </c>
+      <c r="C22" s="10">
+        <v>0</v>
+      </c>
+      <c r="D22" s="10">
+        <v>-1</v>
+      </c>
+      <c r="E22" s="10">
+        <v>-1</v>
+      </c>
+      <c r="F22" s="10">
+        <v>-1</v>
+      </c>
+      <c r="G22" s="10">
+        <v>-1</v>
+      </c>
+      <c r="H22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="I22" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.8571428571428571</v>
+      </c>
+      <c r="J22">
+        <f t="array" ref="J22">MAX(ABS(B22:H22-(ROUND(I22,0))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>190</v>
+      </c>
+      <c r="B23" s="9">
+        <v>1</v>
+      </c>
+      <c r="C23" s="10">
+        <v>2</v>
+      </c>
+      <c r="D23" s="10">
+        <v>2</v>
+      </c>
+      <c r="E23" s="10">
+        <v>2</v>
+      </c>
+      <c r="F23" s="10">
+        <v>1</v>
+      </c>
+      <c r="G23" s="10">
+        <v>1</v>
+      </c>
+      <c r="H23" s="11">
+        <v>1</v>
+      </c>
+      <c r="I23" s="3">
+        <f t="shared" si="0"/>
+        <v>1.4285714285714286</v>
+      </c>
+      <c r="J23">
+        <f t="array" ref="J23">MAX(ABS(B23:H23-(ROUND(I23,0))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>200</v>
+      </c>
+      <c r="B24" s="9">
+        <v>15</v>
+      </c>
+      <c r="C24" s="10">
+        <v>15</v>
+      </c>
+      <c r="D24" s="10">
+        <v>15</v>
+      </c>
+      <c r="E24" s="10">
+        <v>16</v>
+      </c>
+      <c r="F24" s="10">
+        <v>15</v>
+      </c>
+      <c r="G24" s="10">
+        <v>14</v>
+      </c>
+      <c r="H24" s="11">
+        <v>16</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="0"/>
+        <v>15.142857142857142</v>
+      </c>
+      <c r="J24">
+        <f t="array" ref="J24">MAX(ABS(B24:H24-(ROUND(I24,0))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>210</v>
+      </c>
+      <c r="B25" s="9">
+        <v>36</v>
+      </c>
+      <c r="C25" s="10">
+        <v>40</v>
+      </c>
+      <c r="D25" s="10">
+        <v>38</v>
+      </c>
+      <c r="E25" s="10">
+        <v>41</v>
+      </c>
+      <c r="F25" s="10">
+        <v>38</v>
+      </c>
+      <c r="G25" s="10">
+        <v>41</v>
+      </c>
+      <c r="H25" s="11">
+        <v>41</v>
+      </c>
+      <c r="I25" s="3">
+        <f t="shared" si="0"/>
+        <v>39.285714285714285</v>
+      </c>
+      <c r="J25">
+        <f t="array" ref="J25">MAX(ABS(B25:H25-(ROUND(I25,0))))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>220</v>
+      </c>
+      <c r="B26" s="9">
+        <v>67</v>
+      </c>
+      <c r="C26" s="10">
+        <v>71</v>
+      </c>
+      <c r="D26" s="10">
+        <v>69</v>
+      </c>
+      <c r="E26" s="10">
+        <v>71</v>
+      </c>
+      <c r="F26" s="10">
+        <v>70</v>
+      </c>
+      <c r="G26" s="10">
+        <v>68</v>
+      </c>
+      <c r="H26" s="11">
+        <v>74</v>
+      </c>
+      <c r="I26" s="3">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="J26">
+        <f t="array" ref="J26">MAX(ABS(B26:H26-(ROUND(I26,0))))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>230</v>
+      </c>
+      <c r="B27" s="9">
+        <v>102</v>
+      </c>
+      <c r="C27" s="10">
+        <v>103</v>
+      </c>
+      <c r="D27" s="10">
+        <v>101</v>
+      </c>
+      <c r="E27" s="10">
+        <v>101</v>
+      </c>
+      <c r="F27" s="10">
+        <v>99</v>
+      </c>
+      <c r="G27" s="10">
+        <v>106</v>
+      </c>
+      <c r="H27" s="11">
+        <v>105</v>
+      </c>
+      <c r="I27" s="3">
+        <f t="shared" si="0"/>
+        <v>102.42857142857143</v>
+      </c>
+      <c r="J27">
+        <f t="array" ref="J27">MAX(ABS(B27:H27-(ROUND(I27,0))))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>240</v>
+      </c>
+      <c r="B28" s="9">
+        <v>137</v>
+      </c>
+      <c r="C28" s="10">
+        <v>137</v>
+      </c>
+      <c r="D28" s="10">
+        <v>138</v>
+      </c>
+      <c r="E28" s="10">
+        <v>136</v>
+      </c>
+      <c r="F28" s="10">
+        <v>138</v>
+      </c>
+      <c r="G28" s="10">
+        <v>136</v>
+      </c>
+      <c r="H28" s="11">
+        <v>142</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" si="0"/>
+        <v>137.71428571428572</v>
+      </c>
+      <c r="J28">
+        <f t="array" ref="J28">MAX(ABS(B28:H28-(ROUND(I28,0))))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>250</v>
+      </c>
+      <c r="B29" s="9">
+        <v>165</v>
+      </c>
+      <c r="C29" s="10">
+        <v>164</v>
+      </c>
+      <c r="D29" s="10">
+        <v>169</v>
+      </c>
+      <c r="E29" s="10">
+        <v>161</v>
+      </c>
+      <c r="F29" s="10">
+        <v>163</v>
+      </c>
+      <c r="G29" s="10">
+        <v>164</v>
+      </c>
+      <c r="H29" s="11">
+        <v>172</v>
+      </c>
+      <c r="I29" s="3">
+        <f t="shared" si="0"/>
+        <v>165.42857142857142</v>
+      </c>
+      <c r="J29">
+        <f t="array" ref="J29">MAX(ABS(B29:H29-(ROUND(I29,0))))</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>260</v>
+      </c>
+      <c r="B30" s="9">
+        <v>184</v>
+      </c>
+      <c r="C30" s="10">
+        <v>187</v>
+      </c>
+      <c r="D30" s="10">
+        <v>186</v>
+      </c>
+      <c r="E30" s="10">
+        <v>187</v>
+      </c>
+      <c r="F30" s="10">
+        <v>186</v>
+      </c>
+      <c r="G30" s="10">
+        <v>197</v>
+      </c>
+      <c r="H30" s="11">
+        <v>198</v>
+      </c>
+      <c r="I30" s="3">
+        <f t="shared" si="0"/>
+        <v>189.28571428571428</v>
+      </c>
+      <c r="J30">
+        <f t="array" ref="J30">MAX(ABS(B30:H30-(ROUND(I30,0))))</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>270</v>
+      </c>
+      <c r="B31" s="9">
+        <v>198</v>
+      </c>
+      <c r="C31" s="10">
+        <v>198</v>
+      </c>
+      <c r="D31" s="10">
+        <v>198</v>
+      </c>
+      <c r="E31" s="10">
+        <v>198</v>
+      </c>
+      <c r="F31" s="10">
+        <v>198</v>
+      </c>
+      <c r="G31" s="10">
+        <v>217</v>
+      </c>
+      <c r="H31" s="11">
+        <v>211</v>
+      </c>
+      <c r="I31" s="3">
+        <f t="shared" si="0"/>
+        <v>202.57142857142858</v>
+      </c>
+      <c r="J31">
+        <f t="array" ref="J31">MAX(ABS(B31:H31-(ROUND(I31,0))))</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>280</v>
+      </c>
+      <c r="B32" s="9">
+        <v>197</v>
+      </c>
+      <c r="C32" s="10">
+        <v>197</v>
+      </c>
+      <c r="D32" s="10">
+        <v>198</v>
+      </c>
+      <c r="E32" s="10">
+        <v>196</v>
+      </c>
+      <c r="F32" s="10">
+        <v>197</v>
+      </c>
+      <c r="G32" s="10">
+        <v>209</v>
+      </c>
+      <c r="H32" s="11">
+        <v>210</v>
+      </c>
+      <c r="I32" s="3">
+        <f t="shared" si="0"/>
+        <v>200.57142857142858</v>
+      </c>
+      <c r="J32">
+        <f t="array" ref="J32">MAX(ABS(B32:H32-(ROUND(I32,0))))</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>290</v>
+      </c>
+      <c r="B33" s="9">
+        <v>184</v>
+      </c>
+      <c r="C33" s="10">
+        <v>183</v>
+      </c>
+      <c r="D33" s="10">
+        <v>183</v>
+      </c>
+      <c r="E33" s="10">
+        <v>181</v>
+      </c>
+      <c r="F33" s="10">
+        <v>180</v>
+      </c>
+      <c r="G33" s="10">
+        <v>195</v>
+      </c>
+      <c r="H33" s="11">
+        <v>197</v>
+      </c>
+      <c r="I33" s="3">
+        <f t="shared" si="0"/>
+        <v>186.14285714285714</v>
+      </c>
+      <c r="J33">
+        <f t="array" ref="J33">MAX(ABS(B33:H33-(ROUND(I33,0))))</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>300</v>
+      </c>
+      <c r="B34" s="9">
+        <v>158</v>
+      </c>
+      <c r="C34" s="10">
+        <v>157</v>
+      </c>
+      <c r="D34" s="10">
+        <v>158</v>
+      </c>
+      <c r="E34" s="10">
+        <v>155</v>
+      </c>
+      <c r="F34" s="10">
+        <v>157</v>
+      </c>
+      <c r="G34" s="10">
+        <v>168</v>
+      </c>
+      <c r="H34" s="11">
+        <v>170</v>
+      </c>
+      <c r="I34" s="3">
+        <f t="shared" si="0"/>
+        <v>160.42857142857142</v>
+      </c>
+      <c r="J34">
+        <f t="array" ref="J34">MAX(ABS(B34:H34-(ROUND(I34,0))))</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>310</v>
+      </c>
+      <c r="B35" s="9">
+        <v>124</v>
+      </c>
+      <c r="C35" s="10">
+        <v>122</v>
+      </c>
+      <c r="D35" s="10">
+        <v>121</v>
+      </c>
+      <c r="E35" s="10">
+        <v>122</v>
+      </c>
+      <c r="F35" s="10">
+        <v>121</v>
+      </c>
+      <c r="G35" s="10">
+        <v>130</v>
+      </c>
+      <c r="H35" s="11">
+        <v>130</v>
+      </c>
+      <c r="I35" s="3">
+        <f t="shared" si="0"/>
+        <v>124.28571428571429</v>
+      </c>
+      <c r="J35">
+        <f t="array" ref="J35">MAX(ABS(B35:H35-(ROUND(I35,0))))</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>320</v>
+      </c>
+      <c r="B36" s="9">
+        <v>88</v>
+      </c>
+      <c r="C36" s="10">
+        <v>88</v>
+      </c>
+      <c r="D36" s="10">
+        <v>88</v>
+      </c>
+      <c r="E36" s="10">
+        <v>87</v>
+      </c>
+      <c r="F36" s="10">
+        <v>88</v>
+      </c>
+      <c r="G36" s="10">
+        <v>92</v>
+      </c>
+      <c r="H36" s="11">
+        <v>96</v>
+      </c>
+      <c r="I36" s="3">
+        <f t="shared" si="0"/>
+        <v>89.571428571428569</v>
+      </c>
+      <c r="J36">
+        <f t="array" ref="J36">MAX(ABS(B36:H36-(ROUND(I36,0))))</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>330</v>
+      </c>
+      <c r="B37" s="9">
+        <v>54</v>
+      </c>
+      <c r="C37" s="10">
+        <v>54</v>
+      </c>
+      <c r="D37" s="10">
+        <v>52</v>
+      </c>
+      <c r="E37" s="10">
+        <v>55</v>
+      </c>
+      <c r="F37" s="10">
+        <v>55</v>
+      </c>
+      <c r="G37" s="10">
+        <v>56</v>
+      </c>
+      <c r="H37" s="11">
+        <v>57</v>
+      </c>
+      <c r="I37" s="3">
+        <f t="shared" si="0"/>
+        <v>54.714285714285715</v>
+      </c>
+      <c r="J37">
+        <f t="array" ref="J37">MAX(ABS(B37:H37-(ROUND(I37,0))))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>340</v>
+      </c>
+      <c r="B38" s="9">
+        <v>25</v>
+      </c>
+      <c r="C38" s="10">
+        <v>26</v>
+      </c>
+      <c r="D38" s="10">
+        <v>25</v>
+      </c>
+      <c r="E38" s="10">
+        <v>27</v>
+      </c>
+      <c r="F38" s="10">
+        <v>25</v>
+      </c>
+      <c r="G38" s="10">
+        <v>26</v>
+      </c>
+      <c r="H38" s="11">
+        <v>25</v>
+      </c>
+      <c r="I38" s="3">
+        <f t="shared" si="0"/>
+        <v>25.571428571428573</v>
+      </c>
+      <c r="J38">
+        <f t="array" ref="J38">MAX(ABS(B38:H38-(ROUND(I38,0))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>350</v>
+      </c>
+      <c r="B39" s="9">
+        <v>8</v>
+      </c>
+      <c r="C39" s="10">
+        <v>7</v>
+      </c>
+      <c r="D39" s="10">
+        <v>7</v>
+      </c>
+      <c r="E39" s="10">
+        <v>7</v>
+      </c>
+      <c r="F39" s="10">
+        <v>6</v>
+      </c>
+      <c r="G39" s="10">
+        <v>7</v>
+      </c>
+      <c r="H39" s="11">
+        <v>8</v>
+      </c>
+      <c r="I39" s="3">
+        <f t="shared" si="0"/>
+        <v>7.1428571428571432</v>
+      </c>
+      <c r="J39">
+        <f t="array" ref="J39">MAX(ABS(B39:H39-(ROUND(I39,0))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>360</v>
+      </c>
+      <c r="B40" s="12">
+        <v>-1</v>
+      </c>
+      <c r="C40" s="13">
+        <v>-1</v>
+      </c>
+      <c r="D40" s="13">
+        <v>-1</v>
+      </c>
+      <c r="E40" s="13">
+        <v>-1</v>
+      </c>
+      <c r="F40" s="13">
+        <v>-1</v>
+      </c>
+      <c r="G40" s="13">
+        <v>-1</v>
+      </c>
+      <c r="H40" s="14">
+        <v>-1</v>
+      </c>
+      <c r="I40" s="3">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="J40">
+        <f t="array" ref="J40">MAX(ABS(B40:H40-(ROUND(I40,0))))</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>